<commit_message>
best in place added
</commit_message>
<xml_diff>
--- a/roles.xlsx
+++ b/roles.xlsx
@@ -53,7 +53,7 @@
     <t>Gina</t>
   </si>
   <si>
-    <t>Bronco Ernie</t>
+    <t>Bronco</t>
   </si>
   <si>
     <t>Salvatore</t>
@@ -161,7 +161,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D16" activeCellId="0" pane="topLeft" sqref="D16"/>
+      <selection activeCell="B12" activeCellId="0" pane="topLeft" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>

</xml_diff>